<commit_message>
Refactor certificate-sender to track failed email sends and finally create robust node app
</commit_message>
<xml_diff>
--- a/certificate-sender/participants-sample.xlsx
+++ b/certificate-sender/participants-sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Rukshan Fernando\OneDrive\Desktop\My_Portfollio\RealWorlds\HackMoral\Hackmoral-6.0\certificate-sender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b03e12cd552061fc/Desktop/My_Portfollio/RealWorlds/HackMoral/Hackmoral-6.0/certificate-sender/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E2B4F2D-6804-4A38-BDB6-2D20AB82B44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{6E2B4F2D-6804-4A38-BDB6-2D20AB82B44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D55ACCE-58E2-4F81-9796-67B2AC88A557}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C143DF1-C9F5-4F46-84CF-C87CD513F946}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -44,29 +44,17 @@
     <t>Email</t>
   </si>
   <si>
-    <t>Rukshan Fernando</t>
+    <t>Participant Name</t>
   </si>
   <si>
-    <t>Prathibha Dasanayaka</t>
-  </si>
-  <si>
-    <t>Nimesh rukshan Fernando</t>
-  </si>
-  <si>
-    <t>rukshanfernando0416@gmail.com</t>
-  </si>
-  <si>
-    <t>rukshanfernandoeducation123@gmail.com</t>
-  </si>
-  <si>
-    <t>fernandownr.21@itfac.mrt.ac.lk</t>
+    <t>participantEmail@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +66,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1F1F1F"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,15 +99,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF1F1F1F"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -123,6 +138,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28FC2A51-563A-4B88-984D-223BE20C9F9E}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{28FC2A51-563A-4B88-984D-223BE20C9F9E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{362C69DE-8170-4101-8A7B-EEC2F1079301}" name="Name" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{92327506-1C99-4128-9DC6-EF20547BF21C}" name="Email" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFECE68-9961-4519-AE8B-7BDBBB4C2884}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,35 +493,24 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{F0394E84-881C-49E3-9201-1E71E58C9C0B}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{F8C2717B-9A4F-4929-9745-BF369E3C910E}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{57AA56FC-1317-4892-976E-8A37E86D9C9E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>